<commit_message>
Add ed.biordm.sbol.synbio.handler.FeaturesReader for parsing excel file, dependencies in pom.xml and test class
</commit_message>
<xml_diff>
--- a/src/test/resources/ed/biordm/sbol/synbio/handler/update_designs_test.xlsx
+++ b/src/test/resources/ed/biordm/sbol/synbio/handler/update_designs_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Chickens\Documents\EPCC\SynthSys\code_projects\synbio-toolkit\src\test\resources\ed\biordm\sbol\synbio\handler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7124D294-B533-4F04-A0FD-22374A967E7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F088BDC-DA5A-4DD5-B374-690F59DBE0B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>attachment_filename</t>
   </si>
@@ -61,6 +61,21 @@
   </si>
   <si>
     <t>The attached genbank file is from ftp://ftp.ncbi.nlm.nih.gov/genomes/Viruses/abisko_virus_uid399942/NC_035470.gbk</t>
+  </si>
+  <si>
+    <t>0001_slr0611_right</t>
+  </si>
+  <si>
+    <t>this is a row with an empty attachment file</t>
+  </si>
+  <si>
+    <t>NC_014139.gbk</t>
+  </si>
+  <si>
+    <t>This is a row with an empty description</t>
+  </si>
+  <si>
+    <t>0003_slr0613_left</t>
   </si>
 </sst>
 </file>
@@ -378,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W8" sqref="W8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,7 +449,30 @@
         <v>11</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update test/resources/../update_designs_test.xlsx with full file paths for attachment
</commit_message>
<xml_diff>
--- a/src/test/resources/ed/biordm/sbol/synbio/handler/update_designs_test.xlsx
+++ b/src/test/resources/ed/biordm/sbol/synbio/handler/update_designs_test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Chickens\Documents\EPCC\SynthSys\code_projects\synbio-toolkit\src\test\resources\ed\biordm\sbol\synbio\handler\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Chickens\Documents\EPCC\SynthSys\code_projects\synbio-toolkit\target\test-classes\ed\biordm\sbol\synbio\handler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F088BDC-DA5A-4DD5-B374-690F59DBE0B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE5DAEF-4AC5-4FD3-B4B1-32BC4C5BE890}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9045" yWindow="450" windowWidth="14100" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,12 +45,6 @@
     <t>sll0199_right</t>
   </si>
   <si>
-    <t>NC_001499.gbk</t>
-  </si>
-  <si>
-    <t>NC_035470.gbk</t>
-  </si>
-  <si>
     <t>this is the right flank of cyano_codA_Km plasmid</t>
   </si>
   <si>
@@ -69,13 +63,19 @@
     <t>this is a row with an empty attachment file</t>
   </si>
   <si>
-    <t>NC_014139.gbk</t>
-  </si>
-  <si>
     <t>This is a row with an empty description</t>
   </si>
   <si>
     <t>0003_slr0613_left</t>
+  </si>
+  <si>
+    <t>D:\Users\Chickens\Documents\EPCC\SynthSys\code_projects\synbio-toolkit\src\test\resources\ed\biordm\sbol\synbio\handler\NC_035470.gbk</t>
+  </si>
+  <si>
+    <t>D:\Users\Chickens\Documents\EPCC\SynthSys\code_projects\synbio-toolkit\src\test\resources\ed\biordm\sbol\synbio\handler\NC_014139.gbk</t>
+  </si>
+  <si>
+    <t>D:\Users\Chickens\Documents\EPCC\SynthSys\code_projects\synbio-toolkit\src\test\resources\ed\biordm\sbol\synbio\handler\NC_001499.gbk</t>
   </si>
 </sst>
 </file>
@@ -396,7 +396,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,13 +426,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -440,35 +440,35 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>